<commit_message>
feat(administration): admin can create single staff
- fix issues with change password and cron scheduler
- add endpoint for creating a single staff

[Delivers #166336217]
</commit_message>
<xml_diff>
--- a/src/tests/integration/__tests__/testFiles/validExcel.xlsx
+++ b/src/tests/integration/__tests__/testFiles/validExcel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>TN201234</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Damian</t>
   </si>
   <si>
-    <t>Potter</t>
-  </si>
-  <si>
     <t>Latifa.Damian@some.com</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>Dark</t>
   </si>
   <si>
-    <t>Liminade</t>
-  </si>
-  <si>
     <t>Joy.Dark@some.com</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
     <t>Arrow</t>
   </si>
   <si>
-    <t>Franchise</t>
-  </si>
-  <si>
     <t>Soy.Arrow@some.com</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
     <t>Felicity</t>
   </si>
   <si>
-    <t>Bullock</t>
-  </si>
-  <si>
     <t>Boy.Felicity@some.com</t>
   </si>
   <si>
@@ -124,9 +112,6 @@
     <t>Spider</t>
   </si>
   <si>
-    <t>Sadia</t>
-  </si>
-  <si>
     <t>Jaga.Spider@some.com</t>
   </si>
   <si>
@@ -142,9 +127,6 @@
     <t>Cyber</t>
   </si>
   <si>
-    <t>Cruise</t>
-  </si>
-  <si>
     <t>Fray.Cyber@some.com</t>
   </si>
   <si>
@@ -160,9 +142,6 @@
     <t>Crime</t>
   </si>
   <si>
-    <t>Banks</t>
-  </si>
-  <si>
     <t>Broos.Crime@some.com</t>
   </si>
   <si>
@@ -176,9 +155,6 @@
   </si>
   <si>
     <t>Nogood</t>
-  </si>
-  <si>
-    <t>Llyod</t>
   </si>
   <si>
     <t>Brass.Nogood@some.com</t>
@@ -216,12 +192,18 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -234,16 +216,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -253,20 +235,17 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -286,6 +265,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -424,13 +404,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -529,10 +503,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -787,13 +761,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1106,10 +1074,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1363,14 +1331,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="14.5" style="1" customWidth="1"/>
-    <col min="7" max="256" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">
@@ -1389,184 +1357,158 @@
       <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="C2" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="D2" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="E2" t="s" s="3">
         <v>9</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>11</v>
       </c>
     </row>
     <row r="3" ht="14.7" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="D3" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="E3" t="s" s="3">
         <v>14</v>
-      </c>
-      <c r="D3" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>17</v>
       </c>
     </row>
     <row r="4" ht="14.7" customHeight="1">
       <c r="A4" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="E4" t="s" s="3">
         <v>19</v>
-      </c>
-      <c r="C4" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s" s="3">
-        <v>22</v>
       </c>
     </row>
     <row r="5" ht="14.7" customHeight="1">
       <c r="A5" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="E5" t="s" s="3">
         <v>24</v>
-      </c>
-      <c r="C5" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s" s="3">
-        <v>28</v>
       </c>
     </row>
     <row r="6" ht="14.7" customHeight="1">
       <c r="A6" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s" s="3">
         <v>29</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>31</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" t="s" s="3">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s" s="3">
-        <v>33</v>
       </c>
     </row>
     <row r="7" ht="14.7" customHeight="1">
       <c r="A7" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s" s="3">
         <v>34</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s" s="3">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="3">
-        <v>39</v>
       </c>
     </row>
     <row r="8" ht="14.7" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s" s="3">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" ht="14.7" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s" s="3">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s" s="3">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" ht="14.7" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s" s="3">
-        <v>56</v>
-      </c>
-      <c r="F10" t="s" s="3">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>